<commit_message>
fix resolution when printing on A3
</commit_message>
<xml_diff>
--- a/files/resources/Core/templates/AHU/PDF_Print_AHU.xlsx
+++ b/files/resources/Core/templates/AHU/PDF_Print_AHU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DengusiakM\Documents\GitHub\SAM\SAM_UI\files\resources\Core\templates\AHU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0949C0C4-8241-4ABA-A39F-3DDA8325AF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B530D94-0F64-473F-B320-B8A6D0BEDECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D450CF10-0C30-412E-BDB3-053468AC8C92}"/>
   </bookViews>
@@ -1007,7 +1007,7 @@
   <dimension ref="A1:AA146"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A67" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+      <selection activeCell="M82" sqref="M82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5185,8 +5185,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AB98"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A43" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="O57" sqref="O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5222,7 +5222,7 @@
       <c r="S1" s="35"/>
       <c r="T1" s="35"/>
       <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
+      <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
@@ -5252,7 +5252,7 @@
       <c r="S2" s="35"/>
       <c r="T2" s="35"/>
       <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
+      <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -5282,7 +5282,7 @@
       <c r="S3" s="35"/>
       <c r="T3" s="35"/>
       <c r="U3" s="35"/>
-      <c r="V3" s="35"/>
+      <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -5312,7 +5312,7 @@
       <c r="S4" s="35"/>
       <c r="T4" s="35"/>
       <c r="U4" s="35"/>
-      <c r="V4" s="35"/>
+      <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
@@ -5342,7 +5342,7 @@
       <c r="S5" s="35"/>
       <c r="T5" s="35"/>
       <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
+      <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
@@ -5372,7 +5372,7 @@
       <c r="S6" s="35"/>
       <c r="T6" s="35"/>
       <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
+      <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
@@ -5402,7 +5402,7 @@
       <c r="S7" s="35"/>
       <c r="T7" s="35"/>
       <c r="U7" s="35"/>
-      <c r="V7" s="35"/>
+      <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
@@ -5432,7 +5432,7 @@
       <c r="S8" s="35"/>
       <c r="T8" s="35"/>
       <c r="U8" s="35"/>
-      <c r="V8" s="35"/>
+      <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
@@ -5462,7 +5462,7 @@
       <c r="S9" s="35"/>
       <c r="T9" s="35"/>
       <c r="U9" s="35"/>
-      <c r="V9" s="35"/>
+      <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
@@ -5492,7 +5492,7 @@
       <c r="S10" s="35"/>
       <c r="T10" s="35"/>
       <c r="U10" s="35"/>
-      <c r="V10" s="35"/>
+      <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
@@ -5522,7 +5522,7 @@
       <c r="S11" s="35"/>
       <c r="T11" s="35"/>
       <c r="U11" s="35"/>
-      <c r="V11" s="35"/>
+      <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
@@ -5552,7 +5552,7 @@
       <c r="S12" s="35"/>
       <c r="T12" s="35"/>
       <c r="U12" s="35"/>
-      <c r="V12" s="35"/>
+      <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
@@ -5582,7 +5582,7 @@
       <c r="S13" s="35"/>
       <c r="T13" s="35"/>
       <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
+      <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
@@ -5612,7 +5612,7 @@
       <c r="S14" s="35"/>
       <c r="T14" s="35"/>
       <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
+      <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
@@ -5642,7 +5642,7 @@
       <c r="S15" s="35"/>
       <c r="T15" s="35"/>
       <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
+      <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
@@ -5672,7 +5672,7 @@
       <c r="S16" s="35"/>
       <c r="T16" s="35"/>
       <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
+      <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
@@ -5702,7 +5702,7 @@
       <c r="S17" s="35"/>
       <c r="T17" s="35"/>
       <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
+      <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
@@ -5732,7 +5732,7 @@
       <c r="S18" s="35"/>
       <c r="T18" s="35"/>
       <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
+      <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
@@ -5762,7 +5762,7 @@
       <c r="S19" s="35"/>
       <c r="T19" s="35"/>
       <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
+      <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
@@ -5792,7 +5792,7 @@
       <c r="S20" s="35"/>
       <c r="T20" s="35"/>
       <c r="U20" s="35"/>
-      <c r="V20" s="35"/>
+      <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
@@ -5822,7 +5822,7 @@
       <c r="S21" s="35"/>
       <c r="T21" s="35"/>
       <c r="U21" s="35"/>
-      <c r="V21" s="35"/>
+      <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
@@ -5852,7 +5852,7 @@
       <c r="S22" s="35"/>
       <c r="T22" s="35"/>
       <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
+      <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
@@ -5882,7 +5882,7 @@
       <c r="S23" s="35"/>
       <c r="T23" s="35"/>
       <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
+      <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
@@ -5912,7 +5912,7 @@
       <c r="S24" s="35"/>
       <c r="T24" s="35"/>
       <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
+      <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
@@ -5942,7 +5942,7 @@
       <c r="S25" s="35"/>
       <c r="T25" s="35"/>
       <c r="U25" s="35"/>
-      <c r="V25" s="35"/>
+      <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
@@ -5972,7 +5972,7 @@
       <c r="S26" s="35"/>
       <c r="T26" s="35"/>
       <c r="U26" s="35"/>
-      <c r="V26" s="35"/>
+      <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
@@ -6002,7 +6002,7 @@
       <c r="S27" s="35"/>
       <c r="T27" s="35"/>
       <c r="U27" s="35"/>
-      <c r="V27" s="35"/>
+      <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
@@ -6032,7 +6032,7 @@
       <c r="S28" s="35"/>
       <c r="T28" s="35"/>
       <c r="U28" s="35"/>
-      <c r="V28" s="35"/>
+      <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
@@ -6062,7 +6062,7 @@
       <c r="S29" s="35"/>
       <c r="T29" s="35"/>
       <c r="U29" s="35"/>
-      <c r="V29" s="35"/>
+      <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
@@ -6092,7 +6092,7 @@
       <c r="S30" s="35"/>
       <c r="T30" s="35"/>
       <c r="U30" s="35"/>
-      <c r="V30" s="35"/>
+      <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
@@ -6122,7 +6122,7 @@
       <c r="S31" s="35"/>
       <c r="T31" s="35"/>
       <c r="U31" s="35"/>
-      <c r="V31" s="35"/>
+      <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
@@ -6152,7 +6152,7 @@
       <c r="S32" s="35"/>
       <c r="T32" s="35"/>
       <c r="U32" s="35"/>
-      <c r="V32" s="35"/>
+      <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
@@ -6182,7 +6182,7 @@
       <c r="S33" s="35"/>
       <c r="T33" s="35"/>
       <c r="U33" s="35"/>
-      <c r="V33" s="35"/>
+      <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
       <c r="Y33" s="1"/>
@@ -6212,7 +6212,7 @@
       <c r="S34" s="35"/>
       <c r="T34" s="35"/>
       <c r="U34" s="35"/>
-      <c r="V34" s="35"/>
+      <c r="V34" s="1"/>
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
       <c r="Y34" s="1"/>
@@ -6242,7 +6242,7 @@
       <c r="S35" s="35"/>
       <c r="T35" s="35"/>
       <c r="U35" s="35"/>
-      <c r="V35" s="35"/>
+      <c r="V35" s="1"/>
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
@@ -6272,7 +6272,7 @@
       <c r="S36" s="35"/>
       <c r="T36" s="35"/>
       <c r="U36" s="35"/>
-      <c r="V36" s="35"/>
+      <c r="V36" s="1"/>
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
       <c r="Y36" s="1"/>
@@ -6302,7 +6302,7 @@
       <c r="S37" s="35"/>
       <c r="T37" s="35"/>
       <c r="U37" s="35"/>
-      <c r="V37" s="35"/>
+      <c r="V37" s="1"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
       <c r="Y37" s="1"/>
@@ -6332,7 +6332,7 @@
       <c r="S38" s="35"/>
       <c r="T38" s="35"/>
       <c r="U38" s="35"/>
-      <c r="V38" s="35"/>
+      <c r="V38" s="1"/>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
       <c r="Y38" s="1"/>
@@ -6362,7 +6362,7 @@
       <c r="S39" s="35"/>
       <c r="T39" s="35"/>
       <c r="U39" s="35"/>
-      <c r="V39" s="35"/>
+      <c r="V39" s="1"/>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
@@ -6392,7 +6392,7 @@
       <c r="S40" s="35"/>
       <c r="T40" s="35"/>
       <c r="U40" s="35"/>
-      <c r="V40" s="35"/>
+      <c r="V40" s="1"/>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
@@ -6422,7 +6422,7 @@
       <c r="S41" s="35"/>
       <c r="T41" s="35"/>
       <c r="U41" s="35"/>
-      <c r="V41" s="35"/>
+      <c r="V41" s="1"/>
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
@@ -6452,7 +6452,7 @@
       <c r="S42" s="35"/>
       <c r="T42" s="35"/>
       <c r="U42" s="35"/>
-      <c r="V42" s="35"/>
+      <c r="V42" s="1"/>
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
@@ -6482,7 +6482,7 @@
       <c r="S43" s="35"/>
       <c r="T43" s="35"/>
       <c r="U43" s="35"/>
-      <c r="V43" s="35"/>
+      <c r="V43" s="1"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
@@ -6512,7 +6512,7 @@
       <c r="S44" s="35"/>
       <c r="T44" s="35"/>
       <c r="U44" s="35"/>
-      <c r="V44" s="35"/>
+      <c r="V44" s="1"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
@@ -6542,7 +6542,7 @@
       <c r="S45" s="35"/>
       <c r="T45" s="35"/>
       <c r="U45" s="35"/>
-      <c r="V45" s="35"/>
+      <c r="V45" s="1"/>
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
       <c r="Y45" s="1"/>
@@ -6572,7 +6572,7 @@
       <c r="S46" s="35"/>
       <c r="T46" s="35"/>
       <c r="U46" s="35"/>
-      <c r="V46" s="35"/>
+      <c r="V46" s="1"/>
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
       <c r="Y46" s="1"/>
@@ -6602,7 +6602,7 @@
       <c r="S47" s="35"/>
       <c r="T47" s="35"/>
       <c r="U47" s="35"/>
-      <c r="V47" s="35"/>
+      <c r="V47" s="1"/>
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
       <c r="Y47" s="1"/>
@@ -6632,7 +6632,7 @@
       <c r="S48" s="35"/>
       <c r="T48" s="35"/>
       <c r="U48" s="35"/>
-      <c r="V48" s="35"/>
+      <c r="V48" s="1"/>
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
       <c r="Y48" s="1"/>
@@ -6662,7 +6662,7 @@
       <c r="S49" s="35"/>
       <c r="T49" s="35"/>
       <c r="U49" s="35"/>
-      <c r="V49" s="35"/>
+      <c r="V49" s="1"/>
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
       <c r="Y49" s="1"/>
@@ -6692,7 +6692,7 @@
       <c r="S50" s="35"/>
       <c r="T50" s="35"/>
       <c r="U50" s="35"/>
-      <c r="V50" s="35"/>
+      <c r="V50" s="1"/>
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
       <c r="Y50" s="1"/>
@@ -7947,7 +7947,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:V50"/>
+    <mergeCell ref="A1:U50"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="141" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>